<commit_message>
fixed bad commission codes
</commit_message>
<xml_diff>
--- a/Dropship/XY Sense.xlsx
+++ b/Dropship/XY Sense.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Finance\Billing Template\Upstream\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Finance\Billing Template\Upstream\Dropship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFA667D-88FE-4B22-AD18-5FA67733EFA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3773311-A2B8-40BC-B4CE-325C2928E339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00A1F220-B496-4644-BB55-836357F490EA}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00A1F220-B496-4644-BB55-836357F490EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Shipped SKU" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,31 @@
     <sheet name="Type Summary" sheetId="6" r:id="rId5"/>
     <sheet name="Summary" sheetId="10" r:id="rId6"/>
     <sheet name="Errors" sheetId="9" r:id="rId7"/>
+    <sheet name="Materials" sheetId="11" r:id="rId8"/>
+    <sheet name="Types" sheetId="12" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="229">
   <si>
     <t>SKU</t>
   </si>
@@ -543,12 +556,6 @@
     <t>0</t>
   </si>
   <si>
-    <t>238.32</t>
-  </si>
-  <si>
-    <t>56</t>
-  </si>
-  <si>
     <t>Sub-Account Freight Costs</t>
   </si>
   <si>
@@ -682,6 +689,48 @@
   </si>
   <si>
     <t>XY Gateway Extend (Gen 2) 106-1002 BR</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Ordered</t>
+  </si>
+  <si>
+    <t>Fulfilled</t>
+  </si>
+  <si>
+    <t>xy_sense</t>
+  </si>
+  <si>
+    <t>132</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Type Ref</t>
+  </si>
+  <si>
+    <t>Type Name</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -1219,7 +1268,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="10" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1297,17 +1346,9 @@
     <xf numFmtId="49" fontId="9" fillId="5" borderId="4" xfId="10" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="10" applyBorder="1"/>
-    <xf numFmtId="1" fontId="11" fillId="6" borderId="4" xfId="12" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="11" fillId="6" borderId="4" xfId="12" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="11" fillId="6" borderId="4" xfId="12" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="6" borderId="5" xfId="11" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="9" fillId="5" borderId="4" xfId="10" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="5" borderId="4" xfId="10" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1462,8 +1503,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{689FAB5F-4156-4438-87D9-10E7BB3562C6}" name="Ship_SKU" displayName="Ship_SKU" ref="A1:C7" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
-  <autoFilter ref="A1:C7" xr:uid="{689FAB5F-4156-4438-87D9-10E7BB3562C6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{689FAB5F-4156-4438-87D9-10E7BB3562C6}" name="Ship_SKU" displayName="Ship_SKU" ref="A1:C8" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <autoFilter ref="A1:C8" xr:uid="{689FAB5F-4156-4438-87D9-10E7BB3562C6}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{17679FF9-EB04-473B-8F64-EEE76A76A2B2}" name="SKU" dataCellStyle="Normal"/>
     <tableColumn id="2" xr3:uid="{673B8975-D3E3-418C-9C84-52AE2D79D5AE}" name="Qty" dataDxfId="20" dataCellStyle="Normal"/>
@@ -1608,9 +1649,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1648,7 +1689,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1754,7 +1795,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1896,7 +1937,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1910,16 +1951,16 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1930,12 +1971,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
-      <c r="B2">
-        <v>89</v>
+      <c r="B2" s="41">
+        <v>132</v>
       </c>
       <c r="C2" t="str">
         <f>_xlfn.CONCAT(
@@ -1945,12 +1986,12 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="B3" s="41">
+        <v>38</v>
       </c>
       <c r="C3" t="str">
         <f>_xlfn.CONCAT(
@@ -1960,12 +2001,12 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>17</v>
+        <v>27</v>
+      </c>
+      <c r="B4" s="41">
+        <v>11</v>
       </c>
       <c r="C4" t="str">
         <f>_xlfn.CONCAT(
@@ -1975,12 +2016,12 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="B5" s="41">
+        <v>9</v>
       </c>
       <c r="C5" t="str">
         <f>_xlfn.CONCAT(
@@ -1990,12 +2031,12 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>201</v>
-      </c>
-      <c r="B6">
-        <v>10</v>
+        <v>56</v>
+      </c>
+      <c r="B6" s="41">
+        <v>4</v>
       </c>
       <c r="C6" t="str">
         <f>_xlfn.CONCAT(
@@ -2005,12 +2046,12 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="B7" s="41">
+        <v>4</v>
       </c>
       <c r="C7" t="str">
         <f>_xlfn.CONCAT(
@@ -2020,37 +2061,49 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="41">
+        <v>2</v>
+      </c>
+      <c r="C8" s="40" t="str">
+        <f>_xlfn.CONCAT(
+  IF(ISNA(MATCH(Ship_SKU[[#This Row],[SKU]], SKU[SKU], 0)), _xlfn.CONCAT("Missing ", Ship_SKU[[#This Row],[SKU]], " definition"), ""),
+  IF(ISNUMBER(Ship_SKU[[#This Row],[Qty]]), "", "Quantity is not number")
+)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="B2:B7" xr:uid="{FB48059A-80C0-42C2-8C41-BDE827D81EBA}">
+    <dataValidation type="whole" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="B2:B8" xr:uid="{FB48059A-80C0-42C2-8C41-BDE827D81EBA}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -2069,16 +2122,16 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="A3:D3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>153</v>
       </c>
@@ -2086,21 +2139,21 @@
         <v>158</v>
       </c>
       <c r="C1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>146</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>7</v>
+      <c r="B2" s="41">
+        <v>3</v>
+      </c>
+      <c r="C2" s="41">
+        <v>11</v>
       </c>
       <c r="D2" t="str">
         <f>_xlfn.CONCAT(
@@ -2126,25 +2179,25 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -2158,7 +2211,7 @@
         <v>158</v>
       </c>
       <c r="E1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F1" t="s">
         <v>156</v>
@@ -2179,12 +2232,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1200108</v>
       </c>
       <c r="B2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C2" s="19">
         <v>110</v>
@@ -2222,12 +2275,12 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1200109</v>
       </c>
       <c r="B3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C3" s="19">
         <v>180</v>
@@ -2265,12 +2318,12 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4002237</v>
       </c>
       <c r="B4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C4" s="19">
         <v>5.49</v>
@@ -2281,7 +2334,7 @@
       </c>
       <c r="E4" s="8">
         <f>SUMIF(Type[Box Code], Rate[[#This Row],[SAP Code]], Type[Box Qty])</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F4" s="8">
         <f>SUMIF(SKU[Ship Code], Rate[[#This Row],[SAP Code]], SKU[Ship Qty])</f>
@@ -2297,23 +2350,23 @@
       </c>
       <c r="I4" s="7">
         <f>SUM(Rate[[#This Row],[Orders]:[Commissioned]])</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="J4" s="20">
         <f>Rate[[#This Row],[Rate]]*Rate[[#This Row],[Qty]]</f>
-        <v>38.43</v>
+        <v>60.39</v>
       </c>
       <c r="K4" t="str">
         <f>IF(ISNA(MATCH(Rate[[#This Row],[SAP Code]], Summary!A:A, 0)), _xlfn.CONCAT("Missing ", Rate[[#This Row],[SAP Code]], " in summary"), "")</f>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4002238</v>
       </c>
       <c r="B5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C5" s="19">
         <v>3.28</v>
@@ -2351,12 +2404,12 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4002239</v>
       </c>
       <c r="B6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C6" s="19">
         <v>2.48</v>
@@ -2371,7 +2424,7 @@
       </c>
       <c r="F6" s="8">
         <f>SUMIF(SKU[Ship Code], Rate[[#This Row],[SAP Code]], SKU[Ship Qty])</f>
-        <v>157</v>
+        <v>193</v>
       </c>
       <c r="G6" s="8">
         <f>SUMIF(SKU[Kit Code], Rate[[#This Row],[SAP Code]], SKU[Kit Qty])</f>
@@ -2383,23 +2436,23 @@
       </c>
       <c r="I6" s="7">
         <f>SUM(Rate[[#This Row],[Orders]:[Commissioned]])</f>
-        <v>157</v>
+        <v>193</v>
       </c>
       <c r="J6" s="20">
         <f>Rate[[#This Row],[Rate]]*Rate[[#This Row],[Qty]]</f>
-        <v>389.36</v>
+        <v>478.64</v>
       </c>
       <c r="K6" t="str">
         <f>IF(ISNA(MATCH(Rate[[#This Row],[SAP Code]], Summary!A:A, 0)), _xlfn.CONCAT("Missing ", Rate[[#This Row],[SAP Code]], " in summary"), "")</f>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4002240</v>
       </c>
       <c r="B7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C7" s="19">
         <v>1.89</v>
@@ -2418,7 +2471,7 @@
       </c>
       <c r="G7" s="8">
         <f>SUMIF(SKU[Kit Code], Rate[[#This Row],[SAP Code]], SKU[Kit Qty])</f>
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="H7" s="8">
         <f>SUMIF(SKU[Commission Code], Rate[[#This Row],[SAP Code]], SKU[Ship Qty])</f>
@@ -2426,23 +2479,23 @@
       </c>
       <c r="I7" s="7">
         <f>SUM(Rate[[#This Row],[Orders]:[Commissioned]])</f>
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="J7" s="20">
         <f>Rate[[#This Row],[Rate]]*Rate[[#This Row],[Qty]]</f>
-        <v>264.59999999999997</v>
+        <v>304.28999999999996</v>
       </c>
       <c r="K7" t="str">
         <f>IF(ISNA(MATCH(Rate[[#This Row],[SAP Code]], Summary!A:A, 0)), _xlfn.CONCAT("Missing ", Rate[[#This Row],[SAP Code]], " in summary"), "")</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4002242</v>
       </c>
       <c r="B8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C8" s="19">
         <v>10.99</v>
@@ -2465,27 +2518,27 @@
       </c>
       <c r="H8" s="8">
         <f>SUMIF(SKU[Commission Code], Rate[[#This Row],[SAP Code]], SKU[Ship Qty])</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I8" s="7">
         <f>SUM(Rate[[#This Row],[Orders]:[Commissioned]])</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J8" s="20">
         <f>Rate[[#This Row],[Rate]]*Rate[[#This Row],[Qty]]</f>
-        <v>0</v>
+        <v>21.98</v>
       </c>
       <c r="K8" t="str">
         <f>IF(ISNA(MATCH(Rate[[#This Row],[SAP Code]], Summary!A:A, 0)), _xlfn.CONCAT("Missing ", Rate[[#This Row],[SAP Code]], " in summary"), "")</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4002243</v>
       </c>
       <c r="B9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C9" s="19">
         <v>2.95</v>
@@ -2508,27 +2561,27 @@
       </c>
       <c r="H9" s="8">
         <f>SUMIF(SKU[Commission Code], Rate[[#This Row],[SAP Code]], SKU[Ship Qty])</f>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="I9" s="7">
         <f>SUM(Rate[[#This Row],[Orders]:[Commissioned]])</f>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="J9" s="20">
         <f>Rate[[#This Row],[Rate]]*Rate[[#This Row],[Qty]]</f>
-        <v>0</v>
+        <v>112.10000000000001</v>
       </c>
       <c r="K9" t="str">
         <f>IF(ISNA(MATCH(Rate[[#This Row],[SAP Code]], Summary!A:A, 0)), _xlfn.CONCAT("Missing ", Rate[[#This Row],[SAP Code]], " in summary"), "")</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>4002244</v>
       </c>
       <c r="B10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C10" s="19">
         <v>5.57</v>
@@ -2566,12 +2619,12 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>4002276</v>
       </c>
       <c r="B11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C11" s="19">
         <v>14.67</v>
@@ -2609,12 +2662,12 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>4002277</v>
       </c>
       <c r="B12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C12" s="19">
         <v>13.89</v>
@@ -2652,12 +2705,12 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C13" s="19">
         <v>1</v>
@@ -2695,12 +2748,12 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C14" s="19">
         <v>1</v>
@@ -2738,7 +2791,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -2781,13 +2834,13 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I17" s="11" t="s">
         <v>144</v>
       </c>
       <c r="J17" s="20">
         <f>SUM(Rate[Cost])</f>
-        <v>692.39</v>
+        <v>977.4</v>
       </c>
     </row>
   </sheetData>
@@ -2806,27 +2859,27 @@
   </sheetPr>
   <dimension ref="A1:M77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" customWidth="1"/>
-    <col min="8" max="9" width="11.140625" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.44140625" customWidth="1"/>
+    <col min="8" max="9" width="11.109375" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" customWidth="1"/>
+    <col min="12" max="12" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2867,38 +2920,38 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>186</v>
-      </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="41">
-        <f>SUMIF(Ship_SKU[SKU], SKU[[#This Row],[SKU]], Ship_SKU[Qty])</f>
-        <v>7</v>
-      </c>
-      <c r="E2" s="42">
-        <f>IF(SKU[[#This Row],[Ship Code]]="", 0, VLOOKUP(SKU[[#This Row],[Ship Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="39"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="41">
-        <f>SKU[[#This Row],[Ship Qty]]*SKU[[#This Row],[Kit Items]]</f>
-        <v>0</v>
-      </c>
-      <c r="I2" s="42">
-        <f>IF(SKU[[#This Row],[Kit Code]]="", 0, VLOOKUP(SKU[[#This Row],[Kit Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Kit Qty]])</f>
-        <v>0</v>
-      </c>
-      <c r="J2" s="39"/>
-      <c r="K2" s="43">
-        <f>IF(SKU[[#This Row],[Commission Code]]="", 0, VLOOKUP(SKU[[#This Row],[Commission Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
-        <v>0</v>
-      </c>
-      <c r="L2" s="44">
+        <v>184</v>
+      </c>
+      <c r="C2" s="39"/>
+      <c r="D2" s="4">
+        <f>SUMIF(Ship_SKU[SKU], SKU[[#This Row],[SKU]], Ship_SKU[Qty])</f>
+        <v>11</v>
+      </c>
+      <c r="E2" s="5">
+        <f>IF(SKU[[#This Row],[Ship Code]]="", 0, VLOOKUP(SKU[[#This Row],[Ship Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="4">
+        <f>SKU[[#This Row],[Ship Qty]]*SKU[[#This Row],[Kit Items]]</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="5">
+        <f>IF(SKU[[#This Row],[Kit Code]]="", 0, VLOOKUP(SKU[[#This Row],[Kit Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Kit Qty]])</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="6">
+        <f>IF(SKU[[#This Row],[Commission Code]]="", 0, VLOOKUP(SKU[[#This Row],[Commission Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="10">
         <f>SKU[[#This Row],[Ship Cost]]+SKU[[#This Row],[Kit Cost]]+SKU[[#This Row],[Comission Cost]]</f>
         <v>0</v>
       </c>
@@ -2907,23 +2960,23 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C3" s="1">
         <v>4002239</v>
       </c>
       <c r="D3" s="4">
         <f>SUMIF(Ship_SKU[SKU], SKU[[#This Row],[SKU]], Ship_SKU[Qty])</f>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E3" s="5">
         <f>IF(SKU[[#This Row],[Ship Code]]="", 0, VLOOKUP(SKU[[#This Row],[Ship Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
-        <v>42.16</v>
+        <v>0</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="2"/>
@@ -2942,14 +2995,14 @@
       </c>
       <c r="L3" s="10">
         <f>SKU[[#This Row],[Ship Cost]]+SKU[[#This Row],[Kit Cost]]+SKU[[#This Row],[Comission Cost]]</f>
-        <v>42.16</v>
+        <v>0</v>
       </c>
       <c r="M3" t="str">
         <f>IF(OR(ISNA(SKU[[#This Row],[Ship Cost]]), ISNA(SKU[[#This Row],[Kit Cost]]), ISNA(SKU[[#This Row],[Comission Cost]])), "Error Accessing SAP Rate", "")</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -2995,7 +3048,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -3041,7 +3094,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -3087,7 +3140,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -3135,7 +3188,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -3181,44 +3234,44 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>48</v>
       </c>
       <c r="B9" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="39">
-        <v>4002239</v>
-      </c>
-      <c r="D9" s="41">
-        <f>SUMIF(Ship_SKU[SKU], SKU[[#This Row],[SKU]], Ship_SKU[Qty])</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="42">
-        <f>IF(SKU[[#This Row],[Ship Code]]="", 0, VLOOKUP(SKU[[#This Row],[Ship Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="39">
+      <c r="C9" s="1">
+        <v>4002239</v>
+      </c>
+      <c r="D9" s="4">
+        <f>SUMIF(Ship_SKU[SKU], SKU[[#This Row],[SKU]], Ship_SKU[Qty])</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
+        <f>IF(SKU[[#This Row],[Ship Code]]="", 0, VLOOKUP(SKU[[#This Row],[Ship Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
         <v>4002240</v>
       </c>
-      <c r="G9" s="40">
+      <c r="G9" s="2">
         <v>1</v>
       </c>
-      <c r="H9" s="41">
-        <f>SKU[[#This Row],[Ship Qty]]*SKU[[#This Row],[Kit Items]]</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="42">
-        <f>IF(SKU[[#This Row],[Kit Code]]="", 0, VLOOKUP(SKU[[#This Row],[Kit Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Kit Qty]])</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="40"/>
-      <c r="K9" s="42">
-        <f>IF(SKU[[#This Row],[Commission Code]]="", 0, VLOOKUP(SKU[[#This Row],[Commission Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
-        <v>0</v>
-      </c>
-      <c r="L9" s="44">
+      <c r="H9" s="4">
+        <f>SKU[[#This Row],[Ship Qty]]*SKU[[#This Row],[Kit Items]]</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <f>IF(SKU[[#This Row],[Kit Code]]="", 0, VLOOKUP(SKU[[#This Row],[Kit Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Kit Qty]])</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="5">
+        <f>IF(SKU[[#This Row],[Commission Code]]="", 0, VLOOKUP(SKU[[#This Row],[Commission Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="10">
         <f>SKU[[#This Row],[Ship Cost]]+SKU[[#This Row],[Kit Cost]]+SKU[[#This Row],[Comission Cost]]</f>
         <v>0</v>
       </c>
@@ -3227,46 +3280,46 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="39">
-        <v>4002239</v>
-      </c>
-      <c r="D10" s="41">
-        <f>SUMIF(Ship_SKU[SKU], SKU[[#This Row],[SKU]], Ship_SKU[Qty])</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="42">
-        <f>IF(SKU[[#This Row],[Ship Code]]="", 0, VLOOKUP(SKU[[#This Row],[Ship Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="39">
+      <c r="C10" s="1">
+        <v>4002239</v>
+      </c>
+      <c r="D10" s="4">
+        <f>SUMIF(Ship_SKU[SKU], SKU[[#This Row],[SKU]], Ship_SKU[Qty])</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="5">
+        <f>IF(SKU[[#This Row],[Ship Code]]="", 0, VLOOKUP(SKU[[#This Row],[Ship Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
         <v>4002240</v>
       </c>
-      <c r="G10" s="40">
+      <c r="G10" s="2">
         <v>7</v>
       </c>
-      <c r="H10" s="41">
-        <f>SKU[[#This Row],[Ship Qty]]*SKU[[#This Row],[Kit Items]]</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="42">
-        <f>IF(SKU[[#This Row],[Kit Code]]="", 0, VLOOKUP(SKU[[#This Row],[Kit Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Kit Qty]])</f>
-        <v>0</v>
-      </c>
-      <c r="J10" s="40">
+      <c r="H10" s="4">
+        <f>SKU[[#This Row],[Ship Qty]]*SKU[[#This Row],[Kit Items]]</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
+        <f>IF(SKU[[#This Row],[Kit Code]]="", 0, VLOOKUP(SKU[[#This Row],[Kit Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Kit Qty]])</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
         <v>4002276</v>
       </c>
-      <c r="K10" s="42">
-        <f>IF(SKU[[#This Row],[Commission Code]]="", 0, VLOOKUP(SKU[[#This Row],[Commission Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
-        <v>0</v>
-      </c>
-      <c r="L10" s="44">
+      <c r="K10" s="5">
+        <f>IF(SKU[[#This Row],[Commission Code]]="", 0, VLOOKUP(SKU[[#This Row],[Commission Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="10">
         <f>SKU[[#This Row],[Ship Cost]]+SKU[[#This Row],[Kit Cost]]+SKU[[#This Row],[Comission Cost]]</f>
         <v>0</v>
       </c>
@@ -3275,7 +3328,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -3307,7 +3360,7 @@
         <f>IF(SKU[[#This Row],[Kit Code]]="", 0, VLOOKUP(SKU[[#This Row],[Kit Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Kit Qty]])</f>
         <v>0</v>
       </c>
-      <c r="J11" s="40">
+      <c r="J11" s="2">
         <v>4002276</v>
       </c>
       <c r="K11" s="5">
@@ -3323,7 +3376,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -3355,7 +3408,7 @@
         <f>IF(SKU[[#This Row],[Kit Code]]="", 0, VLOOKUP(SKU[[#This Row],[Kit Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Kit Qty]])</f>
         <v>0</v>
       </c>
-      <c r="J12" s="40">
+      <c r="J12" s="2">
         <v>4002276</v>
       </c>
       <c r="K12" s="5">
@@ -3371,9 +3424,9 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B13" t="s">
         <v>55</v>
@@ -3419,7 +3472,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -3467,7 +3520,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -3515,7 +3568,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -3527,11 +3580,11 @@
       </c>
       <c r="D16" s="4">
         <f>SUMIF(Ship_SKU[SKU], SKU[[#This Row],[SKU]], Ship_SKU[Qty])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E16" s="5">
         <f>IF(SKU[[#This Row],[Ship Code]]="", 0, VLOOKUP(SKU[[#This Row],[Ship Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
-        <v>0</v>
+        <v>9.92</v>
       </c>
       <c r="F16" s="1">
         <v>4002240</v>
@@ -3541,11 +3594,11 @@
       </c>
       <c r="H16" s="4">
         <f>SKU[[#This Row],[Ship Qty]]*SKU[[#This Row],[Kit Items]]</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I16" s="5">
         <f>IF(SKU[[#This Row],[Kit Code]]="", 0, VLOOKUP(SKU[[#This Row],[Kit Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Kit Qty]])</f>
-        <v>0</v>
+        <v>7.56</v>
       </c>
       <c r="J16" s="2"/>
       <c r="K16" s="5">
@@ -3554,14 +3607,14 @@
       </c>
       <c r="L16" s="10">
         <f>SKU[[#This Row],[Ship Cost]]+SKU[[#This Row],[Kit Cost]]+SKU[[#This Row],[Comission Cost]]</f>
-        <v>0</v>
+        <v>17.48</v>
       </c>
       <c r="M16" t="str">
         <f>IF(OR(ISNA(SKU[[#This Row],[Ship Cost]]), ISNA(SKU[[#This Row],[Kit Cost]]), ISNA(SKU[[#This Row],[Comission Cost]])), "Error Accessing SAP Rate", "")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -3573,11 +3626,11 @@
       </c>
       <c r="D17" s="4">
         <f>SUMIF(Ship_SKU[SKU], SKU[[#This Row],[SKU]], Ship_SKU[Qty])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E17" s="5">
         <f>IF(SKU[[#This Row],[Ship Code]]="", 0, VLOOKUP(SKU[[#This Row],[Ship Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
-        <v>0</v>
+        <v>9.92</v>
       </c>
       <c r="F17" s="1">
         <v>4002240</v>
@@ -3587,11 +3640,11 @@
       </c>
       <c r="H17" s="4">
         <f>SKU[[#This Row],[Ship Qty]]*SKU[[#This Row],[Kit Items]]</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I17" s="5">
         <f>IF(SKU[[#This Row],[Kit Code]]="", 0, VLOOKUP(SKU[[#This Row],[Kit Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Kit Qty]])</f>
-        <v>0</v>
+        <v>7.56</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="6">
@@ -3600,30 +3653,30 @@
       </c>
       <c r="L17" s="10">
         <f>SKU[[#This Row],[Ship Cost]]+SKU[[#This Row],[Kit Cost]]+SKU[[#This Row],[Comission Cost]]</f>
-        <v>0</v>
+        <v>17.48</v>
       </c>
       <c r="M17" t="str">
         <f>IF(OR(ISNA(SKU[[#This Row],[Ship Cost]]), ISNA(SKU[[#This Row],[Kit Cost]]), ISNA(SKU[[#This Row],[Comission Cost]])), "Error Accessing SAP Rate", "")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B18" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C18" s="1">
         <v>4002239</v>
       </c>
       <c r="D18" s="4">
         <f>SUMIF(Ship_SKU[SKU], SKU[[#This Row],[SKU]], Ship_SKU[Qty])</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E18" s="5">
         <f>IF(SKU[[#This Row],[Ship Code]]="", 0, VLOOKUP(SKU[[#This Row],[Ship Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
-        <v>24.8</v>
+        <v>0</v>
       </c>
       <c r="F18" s="1">
         <v>4002240</v>
@@ -3633,11 +3686,11 @@
       </c>
       <c r="H18" s="4">
         <f>SKU[[#This Row],[Ship Qty]]*SKU[[#This Row],[Kit Items]]</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I18" s="5">
         <f>IF(SKU[[#This Row],[Kit Code]]="", 0, VLOOKUP(SKU[[#This Row],[Kit Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Kit Qty]])</f>
-        <v>18.899999999999999</v>
+        <v>0</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="5">
@@ -3646,14 +3699,14 @@
       </c>
       <c r="L18" s="10">
         <f>SKU[[#This Row],[Ship Cost]]+SKU[[#This Row],[Kit Cost]]+SKU[[#This Row],[Comission Cost]]</f>
-        <v>43.7</v>
+        <v>0</v>
       </c>
       <c r="M18" t="str">
         <f>IF(OR(ISNA(SKU[[#This Row],[Ship Cost]]), ISNA(SKU[[#This Row],[Kit Cost]]), ISNA(SKU[[#This Row],[Comission Cost]])), "Error Accessing SAP Rate", "")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -3699,7 +3752,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -3745,7 +3798,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -3791,7 +3844,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -3837,7 +3890,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>126</v>
       </c>
@@ -3881,7 +3934,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -3925,7 +3978,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -3969,7 +4022,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>68</v>
       </c>
@@ -4013,7 +4066,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -4025,11 +4078,11 @@
       </c>
       <c r="D27" s="4">
         <f>SUMIF(Ship_SKU[SKU], SKU[[#This Row],[SKU]], Ship_SKU[Qty])</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E27" s="5">
         <f>IF(SKU[[#This Row],[Ship Code]]="", 0, VLOOKUP(SKU[[#This Row],[Ship Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
-        <v>0</v>
+        <v>4.96</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="2"/>
@@ -4046,18 +4099,18 @@
       </c>
       <c r="K27" s="6">
         <f>IF(SKU[[#This Row],[Commission Code]]="", 0, VLOOKUP(SKU[[#This Row],[Commission Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
-        <v>0</v>
+        <v>21.98</v>
       </c>
       <c r="L27" s="10">
         <f>SKU[[#This Row],[Ship Cost]]+SKU[[#This Row],[Kit Cost]]+SKU[[#This Row],[Comission Cost]]</f>
-        <v>0</v>
+        <v>26.94</v>
       </c>
       <c r="M27" t="str">
         <f>IF(OR(ISNA(SKU[[#This Row],[Ship Cost]]), ISNA(SKU[[#This Row],[Kit Cost]]), ISNA(SKU[[#This Row],[Comission Cost]])), "Error Accessing SAP Rate", "")</f>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>70</v>
       </c>
@@ -4101,7 +4154,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>72</v>
       </c>
@@ -4145,12 +4198,12 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B30" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C30" s="38">
         <v>4002239</v>
@@ -4189,12 +4242,12 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B31" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C31" s="38">
         <v>4002239</v>
@@ -4233,12 +4286,12 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B32" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C32" s="38">
         <v>4002239</v>
@@ -4277,12 +4330,12 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B33" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C33" s="38">
         <v>4002239</v>
@@ -4321,12 +4374,12 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B34" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C34" s="38">
         <v>4002239</v>
@@ -4365,12 +4418,12 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B35" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C35" s="38">
         <v>4002239</v>
@@ -4409,12 +4462,12 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B36" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C36" s="38">
         <v>4002239</v>
@@ -4453,7 +4506,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>74</v>
       </c>
@@ -4499,7 +4552,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>76</v>
       </c>
@@ -4545,7 +4598,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>78</v>
       </c>
@@ -4591,7 +4644,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>80</v>
       </c>
@@ -4637,7 +4690,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>82</v>
       </c>
@@ -4683,7 +4736,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>84</v>
       </c>
@@ -4729,7 +4782,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>86</v>
       </c>
@@ -4775,7 +4828,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>88</v>
       </c>
@@ -4821,7 +4874,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>90</v>
       </c>
@@ -4867,7 +4920,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>92</v>
       </c>
@@ -4913,7 +4966,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>94</v>
       </c>
@@ -4959,7 +5012,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>14</v>
       </c>
@@ -4971,11 +5024,11 @@
       </c>
       <c r="D48" s="4">
         <f>SUMIF(Ship_SKU[SKU], SKU[[#This Row],[SKU]], Ship_SKU[Qty])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E48" s="5">
         <f>IF(SKU[[#This Row],[Ship Code]]="", 0, VLOOKUP(SKU[[#This Row],[Ship Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
-        <v>0</v>
+        <v>9.92</v>
       </c>
       <c r="F48" s="1">
         <v>4002240</v>
@@ -4985,11 +5038,11 @@
       </c>
       <c r="H48" s="4">
         <f>SKU[[#This Row],[Ship Qty]]*SKU[[#This Row],[Kit Items]]</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I48" s="5">
         <f>IF(SKU[[#This Row],[Kit Code]]="", 0, VLOOKUP(SKU[[#This Row],[Kit Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Kit Qty]])</f>
-        <v>0</v>
+        <v>22.68</v>
       </c>
       <c r="J48" s="2"/>
       <c r="K48" s="5">
@@ -4998,14 +5051,14 @@
       </c>
       <c r="L48" s="10">
         <f>SKU[[#This Row],[Ship Cost]]+SKU[[#This Row],[Kit Cost]]+SKU[[#This Row],[Comission Cost]]</f>
-        <v>0</v>
+        <v>32.6</v>
       </c>
       <c r="M48" t="str">
         <f>IF(OR(ISNA(SKU[[#This Row],[Ship Cost]]), ISNA(SKU[[#This Row],[Kit Cost]]), ISNA(SKU[[#This Row],[Comission Cost]])), "Error Accessing SAP Rate", "")</f>
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>96</v>
       </c>
@@ -5051,7 +5104,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>98</v>
       </c>
@@ -5097,7 +5150,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>100</v>
       </c>
@@ -5143,7 +5196,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>102</v>
       </c>
@@ -5189,7 +5242,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>104</v>
       </c>
@@ -5235,7 +5288,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>106</v>
       </c>
@@ -5281,7 +5334,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>108</v>
       </c>
@@ -5327,7 +5380,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>110</v>
       </c>
@@ -5373,7 +5426,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>112</v>
       </c>
@@ -5419,7 +5472,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>114</v>
       </c>
@@ -5465,7 +5518,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>116</v>
       </c>
@@ -5511,7 +5564,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>118</v>
       </c>
@@ -5557,7 +5610,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>16</v>
       </c>
@@ -5569,11 +5622,11 @@
       </c>
       <c r="D61" s="4">
         <f>SUMIF(Ship_SKU[SKU], SKU[[#This Row],[SKU]], Ship_SKU[Qty])</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E61" s="5">
         <f>IF(SKU[[#This Row],[Ship Code]]="", 0, VLOOKUP(SKU[[#This Row],[Ship Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
-        <v>0</v>
+        <v>22.32</v>
       </c>
       <c r="F61" s="1">
         <v>4002240</v>
@@ -5583,11 +5636,11 @@
       </c>
       <c r="H61" s="4">
         <f>SKU[[#This Row],[Ship Qty]]*SKU[[#This Row],[Kit Items]]</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I61" s="5">
         <f>IF(SKU[[#This Row],[Kit Code]]="", 0, VLOOKUP(SKU[[#This Row],[Kit Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Kit Qty]])</f>
-        <v>0</v>
+        <v>17.009999999999998</v>
       </c>
       <c r="J61" s="2"/>
       <c r="K61" s="5">
@@ -5596,14 +5649,14 @@
       </c>
       <c r="L61" s="10">
         <f>SKU[[#This Row],[Ship Cost]]+SKU[[#This Row],[Kit Cost]]+SKU[[#This Row],[Comission Cost]]</f>
-        <v>0</v>
+        <v>39.33</v>
       </c>
       <c r="M61" t="str">
         <f>IF(OR(ISNA(SKU[[#This Row],[Ship Cost]]), ISNA(SKU[[#This Row],[Kit Cost]]), ISNA(SKU[[#This Row],[Comission Cost]])), "Error Accessing SAP Rate", "")</f>
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>120</v>
       </c>
@@ -5649,12 +5702,12 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>18</v>
       </c>
       <c r="B63" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C63" s="2">
         <v>4002239</v>
@@ -5691,7 +5744,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>19</v>
       </c>
@@ -5739,7 +5792,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>122</v>
       </c>
@@ -5787,7 +5840,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>20</v>
       </c>
@@ -5799,11 +5852,11 @@
       </c>
       <c r="D66" s="4">
         <f>SUMIF(Ship_SKU[SKU], SKU[[#This Row],[SKU]], Ship_SKU[Qty])</f>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E66" s="5">
         <f>IF(SKU[[#This Row],[Ship Code]]="", 0, VLOOKUP(SKU[[#This Row],[Ship Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
-        <v>59.519999999999996</v>
+        <v>0</v>
       </c>
       <c r="F66" s="1">
         <v>4002240</v>
@@ -5813,11 +5866,11 @@
       </c>
       <c r="H66" s="4">
         <f>SKU[[#This Row],[Ship Qty]]*SKU[[#This Row],[Kit Items]]</f>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="I66" s="5">
         <f>IF(SKU[[#This Row],[Kit Code]]="", 0, VLOOKUP(SKU[[#This Row],[Kit Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Kit Qty]])</f>
-        <v>45.36</v>
+        <v>0</v>
       </c>
       <c r="J66" s="2"/>
       <c r="K66" s="5">
@@ -5826,14 +5879,14 @@
       </c>
       <c r="L66" s="10">
         <f>SKU[[#This Row],[Ship Cost]]+SKU[[#This Row],[Kit Cost]]+SKU[[#This Row],[Comission Cost]]</f>
-        <v>104.88</v>
+        <v>0</v>
       </c>
       <c r="M66" t="str">
         <f>IF(OR(ISNA(SKU[[#This Row],[Ship Cost]]), ISNA(SKU[[#This Row],[Kit Cost]]), ISNA(SKU[[#This Row],[Comission Cost]])), "Error Accessing SAP Rate", "")</f>
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>22</v>
       </c>
@@ -5845,11 +5898,11 @@
       </c>
       <c r="D67" s="4">
         <f>SUMIF(Ship_SKU[SKU], SKU[[#This Row],[SKU]], Ship_SKU[Qty])</f>
-        <v>89</v>
+        <v>132</v>
       </c>
       <c r="E67" s="5">
         <f>IF(SKU[[#This Row],[Ship Code]]="", 0, VLOOKUP(SKU[[#This Row],[Ship Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
-        <v>220.72</v>
+        <v>327.36</v>
       </c>
       <c r="F67" s="1">
         <v>4002240</v>
@@ -5859,11 +5912,11 @@
       </c>
       <c r="H67" s="4">
         <f>SKU[[#This Row],[Ship Qty]]*SKU[[#This Row],[Kit Items]]</f>
-        <v>89</v>
+        <v>132</v>
       </c>
       <c r="I67" s="5">
         <f>IF(SKU[[#This Row],[Kit Code]]="", 0, VLOOKUP(SKU[[#This Row],[Kit Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Kit Qty]])</f>
-        <v>168.20999999999998</v>
+        <v>249.48</v>
       </c>
       <c r="J67" s="35"/>
       <c r="K67" s="5">
@@ -5872,19 +5925,19 @@
       </c>
       <c r="L67" s="10">
         <f>SKU[[#This Row],[Ship Cost]]+SKU[[#This Row],[Kit Cost]]+SKU[[#This Row],[Comission Cost]]</f>
-        <v>388.92999999999995</v>
+        <v>576.84</v>
       </c>
       <c r="M67" t="str">
         <f>IF(OR(ISNA(SKU[[#This Row],[Ship Cost]]), ISNA(SKU[[#This Row],[Kit Cost]]), ISNA(SKU[[#This Row],[Comission Cost]])), "Error Accessing SAP Rate", "")</f>
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B68" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C68" s="2">
         <v>4002239</v>
@@ -5925,7 +5978,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>124</v>
       </c>
@@ -5971,23 +6024,23 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>24</v>
       </c>
       <c r="B70" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C70" s="35">
         <v>4002239</v>
       </c>
       <c r="D70" s="33">
         <f>SUMIF(Ship_SKU[SKU], SKU[[#This Row],[SKU]], Ship_SKU[Qty])</f>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E70" s="34">
         <f>IF(SKU[[#This Row],[Ship Code]]="", 0, VLOOKUP(SKU[[#This Row],[Ship Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
-        <v>42.16</v>
+        <v>0</v>
       </c>
       <c r="F70" s="18">
         <v>4002240</v>
@@ -5997,11 +6050,11 @@
       </c>
       <c r="H70" s="33">
         <f>SKU[[#This Row],[Ship Qty]]*SKU[[#This Row],[Kit Items]]</f>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="I70" s="34">
         <f>IF(SKU[[#This Row],[Kit Code]]="", 0, VLOOKUP(SKU[[#This Row],[Kit Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Kit Qty]])</f>
-        <v>32.129999999999995</v>
+        <v>0</v>
       </c>
       <c r="J70" s="18"/>
       <c r="K70" s="36">
@@ -6010,14 +6063,14 @@
       </c>
       <c r="L70" s="37">
         <f>SKU[[#This Row],[Ship Cost]]+SKU[[#This Row],[Kit Cost]]+SKU[[#This Row],[Comission Cost]]</f>
-        <v>74.289999999999992</v>
+        <v>0</v>
       </c>
       <c r="M70" t="str">
         <f>IF(OR(ISNA(SKU[[#This Row],[Ship Cost]]), ISNA(SKU[[#This Row],[Kit Cost]]), ISNA(SKU[[#This Row],[Comission Cost]])), "Error Accessing SAP Rate", "")</f>
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>129</v>
       </c>
@@ -6046,7 +6099,7 @@
         <v>0</v>
       </c>
       <c r="J71" s="1">
-        <v>4002276</v>
+        <v>4002243</v>
       </c>
       <c r="K71" s="6">
         <f>IF(SKU[[#This Row],[Commission Code]]="", 0, VLOOKUP(SKU[[#This Row],[Commission Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
@@ -6061,7 +6114,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>131</v>
       </c>
@@ -6090,7 +6143,7 @@
         <v>0</v>
       </c>
       <c r="J72" s="1">
-        <v>4002276</v>
+        <v>4002243</v>
       </c>
       <c r="K72" s="6">
         <f>IF(SKU[[#This Row],[Commission Code]]="", 0, VLOOKUP(SKU[[#This Row],[Commission Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
@@ -6105,7 +6158,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>133</v>
       </c>
@@ -6134,7 +6187,7 @@
         <v>0</v>
       </c>
       <c r="J73" s="1">
-        <v>4002276</v>
+        <v>4002243</v>
       </c>
       <c r="K73" s="6">
         <f>IF(SKU[[#This Row],[Commission Code]]="", 0, VLOOKUP(SKU[[#This Row],[Commission Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
@@ -6149,7 +6202,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>135</v>
       </c>
@@ -6178,7 +6231,7 @@
         <v>0</v>
       </c>
       <c r="J74" s="1">
-        <v>4002276</v>
+        <v>4002243</v>
       </c>
       <c r="K74" s="6">
         <f>IF(SKU[[#This Row],[Commission Code]]="", 0, VLOOKUP(SKU[[#This Row],[Commission Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
@@ -6193,7 +6246,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>25</v>
       </c>
@@ -6205,11 +6258,11 @@
       </c>
       <c r="D75" s="4">
         <f>SUMIF(Ship_SKU[SKU], SKU[[#This Row],[SKU]], Ship_SKU[Qty])</f>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="E75" s="5">
         <f>IF(SKU[[#This Row],[Ship Code]]="", 0, VLOOKUP(SKU[[#This Row],[Ship Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
-        <v>0</v>
+        <v>94.24</v>
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="2"/>
@@ -6222,22 +6275,22 @@
         <v>0</v>
       </c>
       <c r="J75" s="1">
-        <v>4002276</v>
+        <v>4002243</v>
       </c>
       <c r="K75" s="6">
         <f>IF(SKU[[#This Row],[Commission Code]]="", 0, VLOOKUP(SKU[[#This Row],[Commission Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
-        <v>0</v>
+        <v>112.10000000000001</v>
       </c>
       <c r="L75" s="10">
         <f>SKU[[#This Row],[Ship Cost]]+SKU[[#This Row],[Kit Cost]]+SKU[[#This Row],[Comission Cost]]</f>
-        <v>0</v>
+        <v>206.34</v>
       </c>
       <c r="M75" t="str">
         <f>IF(OR(ISNA(SKU[[#This Row],[Ship Cost]]), ISNA(SKU[[#This Row],[Kit Cost]]), ISNA(SKU[[#This Row],[Comission Cost]])), "Error Accessing SAP Rate", "")</f>
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>137</v>
       </c>
@@ -6266,7 +6319,7 @@
         <v>0</v>
       </c>
       <c r="J76" s="1">
-        <v>4002276</v>
+        <v>4002243</v>
       </c>
       <c r="K76" s="6">
         <f>IF(SKU[[#This Row],[Commission Code]]="", 0, VLOOKUP(SKU[[#This Row],[Commission Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
@@ -6281,7 +6334,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>139</v>
       </c>
@@ -6309,8 +6362,8 @@
         <f>IF(SKU[[#This Row],[Kit Code]]="", 0, VLOOKUP(SKU[[#This Row],[Kit Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Kit Qty]])</f>
         <v>0</v>
       </c>
-      <c r="J77" s="18">
-        <v>4002276</v>
+      <c r="J77" s="1">
+        <v>4002243</v>
       </c>
       <c r="K77" s="36">
         <f>IF(SKU[[#This Row],[Commission Code]]="", 0, VLOOKUP(SKU[[#This Row],[Commission Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</f>
@@ -6344,20 +6397,20 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>153</v>
       </c>
@@ -6374,13 +6427,13 @@
         <v>141</v>
       </c>
       <c r="F1" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="H1" s="17" t="s">
         <v>197</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>199</v>
       </c>
       <c r="I1" s="17" t="s">
         <v>154</v>
@@ -6389,7 +6442,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>145</v>
       </c>
@@ -6425,7 +6478,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>146</v>
       </c>
@@ -6435,7 +6488,7 @@
       <c r="C3" s="2"/>
       <c r="D3" s="8">
         <f>SUMIF(Ship_Type[REF], Type[[#This Row],[REF]], Ship_Type[Orders])</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3" s="20">
         <f>IF(Type[[#This Row],[Ship Code]]="", 0, VLOOKUP(Type[[#This Row],[Ship Code]], Rate[], 3, FALSE)*Type[[#This Row],[Ship Qty]])</f>
@@ -6446,22 +6499,22 @@
       </c>
       <c r="G3" s="8">
         <f>SUMIF(Ship_Type[REF], Type[[#This Row],[REF]], Ship_Type[Boxes])</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H3" s="20">
         <f>IF(Type[[#This Row],[Box Code]]="", 0, VLOOKUP(Type[[#This Row],[Box Code]], Rate[], 3, FALSE)*Type[[#This Row],[Box Qty]])</f>
-        <v>38.43</v>
+        <v>60.39</v>
       </c>
       <c r="I3" s="10">
         <f>SUM(Type[[#This Row],[Ship Cost]], Type[[#This Row],[Box Cost]])</f>
-        <v>38.43</v>
+        <v>60.39</v>
       </c>
       <c r="J3" t="str">
         <f>IF(OR(ISNA(Type[[#This Row],[Ship Cost]]), ISNA(Type[[#This Row],[Box Cost]])), "Error Accessing SAP Rate", "")</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>147</v>
       </c>
@@ -6497,7 +6550,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>148</v>
       </c>
@@ -6549,18 +6602,18 @@
   </sheetPr>
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>28</v>
       </c>
@@ -6577,16 +6630,16 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="23"/>
       <c r="B2" s="24" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C2" s="25"/>
       <c r="D2" s="26"/>
       <c r="E2" s="25"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="17">
         <v>4002240</v>
       </c>
@@ -6600,28 +6653,28 @@
       </c>
       <c r="D3" s="31">
         <f>VLOOKUP($A3, Rate[[SAP Code]:[Qty]], 9, FALSE)</f>
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="E3">
         <f>C3*D3</f>
-        <v>264.59999999999997</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>304.28999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C4" s="19"/>
       <c r="D4" s="16"/>
       <c r="E4" s="19"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="23"/>
       <c r="B5" s="24" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C5" s="25"/>
       <c r="D5" s="26"/>
       <c r="E5" s="25"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="17">
         <v>4002242</v>
       </c>
@@ -6635,14 +6688,14 @@
       </c>
       <c r="D6" s="31">
         <f>VLOOKUP($A6, Rate[[SAP Code]:[Qty]], 9, FALSE)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E6" s="19">
         <f>C6*D6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>21.98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="30">
         <v>4002243</v>
       </c>
@@ -6656,14 +6709,14 @@
       </c>
       <c r="D7" s="32">
         <f>VLOOKUP($A7, Rate[[SAP Code]:[Qty]], 9, FALSE)</f>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="E7" s="21">
         <f>C7*D7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>112.10000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="17">
         <v>4002276</v>
       </c>
@@ -6684,7 +6737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="30">
         <v>4002277</v>
       </c>
@@ -6705,21 +6758,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C10" s="19"/>
       <c r="D10" s="16"/>
       <c r="E10" s="19"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="23"/>
       <c r="B11" s="24" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C11" s="23"/>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="17">
         <v>4002237</v>
       </c>
@@ -6733,14 +6786,14 @@
       </c>
       <c r="D12" s="31">
         <f>VLOOKUP($A12, Rate[[SAP Code]:[Qty]], 9, FALSE)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E12" s="19">
         <f>C12*D12</f>
-        <v>38.43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>60.39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="30">
         <v>4002238</v>
       </c>
@@ -6761,7 +6814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="17">
         <v>4002239</v>
       </c>
@@ -6775,28 +6828,28 @@
       </c>
       <c r="D14" s="31">
         <f>VLOOKUP($A14, Rate[[SAP Code]:[Qty]], 9, FALSE)</f>
-        <v>157</v>
+        <v>193</v>
       </c>
       <c r="E14" s="19">
         <f>C14*D14</f>
-        <v>389.36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>478.64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C15" s="19"/>
       <c r="D15" s="16"/>
       <c r="E15" s="19"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="24"/>
       <c r="B16" s="24" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C16" s="27"/>
       <c r="D16" s="28"/>
       <c r="E16" s="27"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="17">
         <v>4002244</v>
       </c>
@@ -6817,21 +6870,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C18" s="19"/>
       <c r="D18" s="16"/>
       <c r="E18" s="19"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="24"/>
       <c r="B19" s="24" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C19" s="29"/>
       <c r="D19" s="28"/>
       <c r="E19" s="29"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>30</v>
       </c>
@@ -6844,14 +6897,14 @@
         <v>6.2</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E20">
         <f>C20*D20</f>
-        <v>347.2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="30" t="s">
         <v>32</v>
       </c>
@@ -6872,7 +6925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
         <v>33</v>
       </c>
@@ -6885,14 +6938,14 @@
         <v>1</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E22">
         <f>C22*D22</f>
-        <v>238.32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="30">
         <v>1200108</v>
       </c>
@@ -6912,7 +6965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="17">
         <v>1200109</v>
       </c>
@@ -6932,13 +6985,13 @@
         <v>180</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D26" s="22" t="s">
         <v>144</v>
       </c>
       <c r="E26" s="10">
         <f>SUM(E2:E24)</f>
-        <v>1457.9099999999999</v>
+        <v>1157.4000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -6957,13 +7010,13 @@
       <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>161</v>
       </c>
@@ -6971,7 +7024,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>162</v>
       </c>
@@ -6980,16 +7033,16 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="B3" s="12" t="e">
+      <c r="B3" s="12" t="str">
         <f>_xlfn.IFNA(INDEX(Ship_Type[Error],MATCH(TRUE,INDEX(Ship_Type[Error]&lt;&gt;"",0),0)), "")</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>164</v>
       </c>
@@ -6998,7 +7051,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>165</v>
       </c>
@@ -7007,7 +7060,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>168</v>
       </c>
@@ -7020,4 +7073,199 @@
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEAEFA37-1249-44E0-8CB6-E9149B8FA4EB}">
+  <sheetPr>
+    <tabColor theme="2" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>223</v>
+      </c>
+      <c r="D5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>219</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>219</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>224</v>
+      </c>
+      <c r="D7" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>225</v>
+      </c>
+      <c r="D8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07007CF9-370F-4524-A0CE-FD0AAB0879C1}">
+  <sheetPr>
+    <tabColor theme="2" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>